<commit_message>
issue has been fixed
</commit_message>
<xml_diff>
--- a/participant-manager/src/assets/Email_Import_Template.xlsx
+++ b/participant-manager/src/assets/Email_Import_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prakash\Desktop\uploadExcelsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Firdose\Documents\Github-fda-mystudies\participant-manager\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C4345A-50E7-412C-B138-D1CCB6A2CFBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="7590"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,47 +20,27 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>SL No.</t>
   </si>
   <si>
     <t>Email Address</t>
   </si>
-  <si>
-    <t>prsad2@grr.la</t>
-  </si>
-  <si>
-    <t>prak5@grr.la</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,17 +69,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,11 +388,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,24 +409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>